<commit_message>
Added Wrong Logout URL to verify logout screenshot Assert added with wrong URL
</commit_message>
<xml_diff>
--- a/bin/XLSFiles/TestData.xlsx
+++ b/bin/XLSFiles/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14580" windowHeight="6420" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13185" windowHeight="3990"/>
   </bookViews>
   <sheets>
     <sheet name="LogInData" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="View_ADD_EMP" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:J20"/>
+  <oleSize ref="A1:M10"/>
 </workbook>
 </file>
 
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -728,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>